<commit_message>
Slight change to the table
</commit_message>
<xml_diff>
--- a/Message Structures.xlsx
+++ b/Message Structures.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Darren\Documents\GitHub\ElevatorControlSystem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{31EB15AB-DA48-4CD5-84DD-A51B41973535}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7396985E-80E4-4EE8-BACE-7F1AF55809DE}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12165" xr2:uid="{F76DA7DB-E61D-479D-8310-372DF38C81BC}"/>
   </bookViews>
@@ -85,7 +85,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="45">
   <si>
     <t>Scenario</t>
   </si>
@@ -219,13 +219,37 @@
   <si>
     <t>Message Direction
 (Origin -&gt; Destination)</t>
+  </si>
+  <si>
+    <r>
+      <t>Origin Floor</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="5" tint="-0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Elevator</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -241,23 +265,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="9" tint="-0.249977111117893"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -283,6 +295,12 @@
     <font>
       <sz val="11"/>
       <color theme="7" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -334,22 +352,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
@@ -358,23 +364,35 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -719,7 +737,7 @@
   <dimension ref="A1:M15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -728,7 +746,7 @@
     <col min="3" max="3" width="37.140625" style="1" customWidth="1"/>
     <col min="4" max="4" width="16" style="1" customWidth="1"/>
     <col min="5" max="5" width="17.5703125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="17.140625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="22.42578125" style="1" customWidth="1"/>
     <col min="7" max="7" width="18.28515625" style="1" customWidth="1"/>
     <col min="8" max="8" width="27.7109375" style="1" customWidth="1"/>
     <col min="9" max="11" width="9.140625" style="1"/>
@@ -738,13 +756,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="10"/>
+      <c r="A1" s="6"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C3" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="13" t="s">
+      <c r="D3" s="17" t="s">
         <v>42</v>
       </c>
       <c r="E3" s="12" t="s">
@@ -756,13 +774,13 @@
       <c r="G3" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="H3" s="13" t="s">
+      <c r="H3" s="17" t="s">
         <v>43</v>
       </c>
       <c r="L3" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="M3" s="11"/>
+      <c r="M3" s="7"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C4" s="12"/>
@@ -771,10 +789,10 @@
       <c r="F4" s="12"/>
       <c r="G4" s="12"/>
       <c r="H4" s="12"/>
-      <c r="L4" s="4" t="s">
+      <c r="L4" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="M4" s="11" t="s">
+      <c r="M4" s="7" t="s">
         <v>22</v>
       </c>
     </row>
@@ -797,8 +815,8 @@
       <c r="H5" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="L5" s="4"/>
-      <c r="M5" s="11" t="s">
+      <c r="L5" s="13"/>
+      <c r="M5" s="7" t="s">
         <v>23</v>
       </c>
     </row>
@@ -809,20 +827,20 @@
       <c r="D6" s="3">
         <v>1</v>
       </c>
-      <c r="E6" s="14" t="s">
+      <c r="E6" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="F6" s="6" t="s">
+      <c r="F6" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="G6" s="6" t="s">
+      <c r="G6" s="4" t="s">
         <v>9</v>
       </c>
       <c r="H6" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="L6" s="4"/>
-      <c r="M6" s="11" t="s">
+      <c r="L6" s="13"/>
+      <c r="M6" s="7" t="s">
         <v>24</v>
       </c>
     </row>
@@ -833,11 +851,11 @@
       <c r="D7" s="3">
         <v>2</v>
       </c>
-      <c r="E7" s="15" t="s">
+      <c r="E7" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="F7" s="6" t="s">
-        <v>8</v>
+      <c r="F7" s="4" t="s">
+        <v>44</v>
       </c>
       <c r="G7" s="3">
         <v>0</v>
@@ -845,8 +863,8 @@
       <c r="H7" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="L7" s="4"/>
-      <c r="M7" s="11" t="s">
+      <c r="L7" s="13"/>
+      <c r="M7" s="7" t="s">
         <v>25</v>
       </c>
     </row>
@@ -857,22 +875,22 @@
       <c r="D8" s="3">
         <v>3</v>
       </c>
-      <c r="E8" s="16" t="s">
+      <c r="E8" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="F8" s="6" t="s">
+      <c r="F8" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="G8" s="7" t="s">
+      <c r="G8" s="5" t="s">
         <v>14</v>
       </c>
       <c r="H8" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="L8" s="5" t="s">
+      <c r="L8" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="M8" s="11" t="s">
+      <c r="M8" s="7" t="s">
         <v>26</v>
       </c>
     </row>
@@ -883,20 +901,20 @@
       <c r="D9" s="3">
         <v>4</v>
       </c>
-      <c r="E9" s="17" t="s">
+      <c r="E9" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="F9" s="7" t="s">
+      <c r="F9" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="G9" s="6" t="s">
+      <c r="G9" s="4" t="s">
         <v>9</v>
       </c>
       <c r="H9" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="L9" s="5"/>
-      <c r="M9" s="11" t="s">
+      <c r="L9" s="14"/>
+      <c r="M9" s="7" t="s">
         <v>27</v>
       </c>
     </row>
@@ -907,7 +925,7 @@
       <c r="D10" s="3">
         <v>5</v>
       </c>
-      <c r="E10" s="7" t="s">
+      <c r="E10" s="5" t="s">
         <v>14</v>
       </c>
       <c r="F10" s="3">
@@ -919,10 +937,10 @@
       <c r="H10" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="L10" s="6" t="s">
+      <c r="L10" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="M10" s="11" t="s">
+      <c r="M10" s="7" t="s">
         <v>30</v>
       </c>
     </row>
@@ -933,22 +951,22 @@
       <c r="D11" s="3">
         <v>6</v>
       </c>
-      <c r="E11" s="15" t="s">
+      <c r="E11" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="F11" s="7" t="s">
+      <c r="F11" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="G11" s="6" t="s">
+      <c r="G11" s="4" t="s">
         <v>15</v>
       </c>
       <c r="H11" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="L11" s="7" t="s">
+      <c r="L11" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="M11" s="11" t="s">
+      <c r="M11" s="7" t="s">
         <v>29</v>
       </c>
     </row>
@@ -959,42 +977,42 @@
       <c r="D12" s="3">
         <v>7</v>
       </c>
-      <c r="E12" s="14" t="s">
+      <c r="E12" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="F12" s="6" t="s">
+      <c r="F12" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="G12" s="7" t="s">
+      <c r="G12" s="5" t="s">
         <v>14</v>
       </c>
       <c r="H12" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="L12" s="8" t="s">
+      <c r="L12" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="M12" s="11" t="s">
+      <c r="M12" s="7" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="L13" s="8"/>
-      <c r="M13" s="11" t="s">
+      <c r="L13" s="15"/>
+      <c r="M13" s="7" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="L14" s="9" t="s">
+      <c r="L14" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="M14" s="11" t="s">
+      <c r="M14" s="7" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="L15" s="9"/>
-      <c r="M15" s="11" t="s">
+      <c r="L15" s="16"/>
+      <c r="M15" s="7" t="s">
         <v>34</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Directions and message change
New directions methods to convert direction values to their flag value
for messages
Updated the message format to be more consistent
</commit_message>
<xml_diff>
--- a/Message Structures.xlsx
+++ b/Message Structures.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Darren\Documents\GitHub\ElevatorControlSystem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{021A6E29-4F13-43FD-9640-993460842720}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B60CECF0-0D1F-4ACC-AE5E-45F448C21460}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12165" xr2:uid="{F76DA7DB-E61D-479D-8310-372DF38C81BC}"/>
   </bookViews>
@@ -85,7 +85,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="50">
   <si>
     <t>Scenario</t>
   </si>
@@ -221,30 +221,6 @@
 (Origin -&gt; Destination)</t>
   </si>
   <si>
-    <r>
-      <t>Origin Floor</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>/</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="5" tint="-0.249977111117893"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Elevator</t>
-    </r>
-  </si>
-  <si>
     <t>Empty</t>
   </si>
   <si>
@@ -252,13 +228,22 @@
   </si>
   <si>
     <t>Undecided Values (Will eventually pertain to a specific code)</t>
+  </si>
+  <si>
+    <t>Origin Floor*</t>
+  </si>
+  <si>
+    <t>Elevator*</t>
+  </si>
+  <si>
+    <t>* Only 1 of the two, the other being Empty</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -304,12 +289,6 @@
     <font>
       <sz val="11"/>
       <color theme="7" tint="-0.249977111117893"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -397,6 +376,12 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -414,12 +399,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -764,7 +743,7 @@
   <dimension ref="A1:M17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -786,22 +765,22 @@
       <c r="A1" s="6"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="C3" s="12" t="s">
+      <c r="C3" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="17" t="s">
+      <c r="D3" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="E3" s="12" t="s">
+      <c r="E3" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="F3" s="12" t="s">
+      <c r="F3" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="G3" s="12" t="s">
+      <c r="G3" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="H3" s="17" t="s">
+      <c r="H3" s="19" t="s">
         <v>43</v>
       </c>
       <c r="L3" s="3" t="s">
@@ -810,13 +789,13 @@
       <c r="M3" s="7"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="C4" s="12"/>
-      <c r="D4" s="12"/>
-      <c r="E4" s="12"/>
-      <c r="F4" s="12"/>
-      <c r="G4" s="12"/>
-      <c r="H4" s="12"/>
-      <c r="L4" s="13" t="s">
+      <c r="C4" s="14"/>
+      <c r="D4" s="14"/>
+      <c r="E4" s="14"/>
+      <c r="F4" s="14"/>
+      <c r="G4" s="14"/>
+      <c r="H4" s="14"/>
+      <c r="L4" s="15" t="s">
         <v>7</v>
       </c>
       <c r="M4" s="7" t="s">
@@ -830,19 +809,19 @@
       <c r="D5" s="3">
         <v>0</v>
       </c>
-      <c r="E5" s="19" t="s">
+      <c r="E5" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="F5" s="19" t="s">
+      <c r="F5" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="G5" s="19" t="s">
+      <c r="G5" s="13" t="s">
         <v>6</v>
       </c>
       <c r="H5" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="L5" s="13"/>
+      <c r="L5" s="15"/>
       <c r="M5" s="7" t="s">
         <v>23</v>
       </c>
@@ -866,7 +845,7 @@
       <c r="H6" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="L6" s="13"/>
+      <c r="L6" s="15"/>
       <c r="M6" s="7" t="s">
         <v>24</v>
       </c>
@@ -882,15 +861,15 @@
         <v>10</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="G7" s="18" t="s">
-        <v>45</v>
+        <v>47</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>48</v>
       </c>
       <c r="H7" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="L7" s="13"/>
+      <c r="L7" s="15"/>
       <c r="M7" s="7" t="s">
         <v>25</v>
       </c>
@@ -914,7 +893,7 @@
       <c r="H8" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="L8" s="14" t="s">
+      <c r="L8" s="16" t="s">
         <v>10</v>
       </c>
       <c r="M8" s="7" t="s">
@@ -931,16 +910,16 @@
       <c r="E9" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="F9" s="5" t="s">
+      <c r="F9" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G9" s="5" t="s">
         <v>14</v>
-      </c>
-      <c r="G9" s="4" t="s">
-        <v>9</v>
       </c>
       <c r="H9" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="L9" s="14"/>
+      <c r="L9" s="16"/>
       <c r="M9" s="7" t="s">
         <v>27</v>
       </c>
@@ -952,14 +931,14 @@
       <c r="D10" s="3">
         <v>5</v>
       </c>
-      <c r="E10" s="5" t="s">
+      <c r="E10" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="F10" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="G10" s="5" t="s">
         <v>14</v>
-      </c>
-      <c r="F10" s="18" t="s">
-        <v>45</v>
-      </c>
-      <c r="G10" s="18" t="s">
-        <v>45</v>
       </c>
       <c r="H10" s="3" t="s">
         <v>41</v>
@@ -981,11 +960,11 @@
       <c r="E11" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="F11" s="5" t="s">
+      <c r="F11" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G11" s="5" t="s">
         <v>14</v>
-      </c>
-      <c r="G11" s="4" t="s">
-        <v>15</v>
       </c>
       <c r="H11" s="3" t="s">
         <v>37</v>
@@ -1016,7 +995,7 @@
       <c r="H12" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="L12" s="15" t="s">
+      <c r="L12" s="17" t="s">
         <v>12</v>
       </c>
       <c r="M12" s="7" t="s">
@@ -1024,13 +1003,16 @@
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="L13" s="15"/>
+      <c r="L13" s="17"/>
       <c r="M13" s="7" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="L14" s="16" t="s">
+      <c r="F14" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="L14" s="18" t="s">
         <v>13</v>
       </c>
       <c r="M14" s="7" t="s">
@@ -1038,25 +1020,25 @@
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="L15" s="16"/>
+      <c r="L15" s="18"/>
       <c r="M15" s="7" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="L16" s="18" t="s">
+      <c r="L16" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="M16" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="M16" s="7" t="s">
+    </row>
+    <row r="17" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L17" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="M17" s="7" t="s">
         <v>46</v>
-      </c>
-    </row>
-    <row r="17" spans="12:13" x14ac:dyDescent="0.25">
-      <c r="L17" s="19" t="s">
-        <v>6</v>
-      </c>
-      <c r="M17" s="7" t="s">
-        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>